<commit_message>
Grupos' form working dinamically
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A27BD3-6FD2-5D49-8E32-33C88288BFA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF22FAC-9A46-854D-9B01-179D72911E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,7 +849,7 @@
     <t>Bono 1</t>
   </si>
   <si>
-    <t>2014-10 Prueba 2</t>
+    <t>2014-10 Prueba 3</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Grupos now are being added to the db correctly. Also, some links were fixed and minor style changes
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF22FAC-9A46-854D-9B01-179D72911E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD136C-FEA7-8640-922F-7C3F36D5466D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,7 +849,7 @@
     <t>Bono 1</t>
   </si>
   <si>
-    <t>2014-10 Prueba 3</t>
+    <t>2014-10 Prueba 2</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Changes in Estudiantes list, the way it looks and in Grupos style.
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BD136C-FEA7-8640-922F-7C3F36D5466D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DCE096-9D83-654F-87D7-3B535FFAA48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,7 +849,7 @@
     <t>Bono 1</t>
   </si>
   <si>
-    <t>2014-10 Prueba 2</t>
+    <t>2014-10 Prueba 3</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1201,7 @@
   <dimension ref="A1:K437"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1275,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
When grading the actividad shows the current grade and a completed status
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BCCB87-1E07-7A44-AA1A-B1951988DBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DC562C-8D82-2E43-8894-CF5D2229F5AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>202020</v>
+        <v>201920</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Profesores and Asistentes now can be added to the team
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DC562C-8D82-2E43-8894-CF5D2229F5AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962D4D1A-FB21-FD4F-8537-55F2D01A2463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:K433"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>201920</v>
+        <v>202010</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
1 bug when grading fixed. Variaciones selected now persisted
</commit_message>
<xml_diff>
--- a/Herramienta/static/files/Actividad.xlsx
+++ b/Herramienta/static/files/Actividad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laiton/Desktop/Universidad/TesisIIND/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9606CC18-C31C-954A-BF23-977B9735BF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6973F258-49F8-134B-94F4-8820B08F2FE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="267">
   <si>
     <t>Nombre:</t>
   </si>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:K432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1636,6 +1636,9 @@
       <c r="A30">
         <v>3</v>
       </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31">

</xml_diff>